<commit_message>
Ran regression model w/ Siegel ownership rate
</commit_message>
<xml_diff>
--- a/data_edited/gun_ownership_rates_2013.xlsx
+++ b/data_edited/gun_ownership_rates_2013.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF487CB5-4991-487F-B6BD-0FCC1CC5A8A4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A4A548-5095-4187-87D6-2ADE222C41C7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1831,14 +1831,8 @@
       <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F53" s="1">
-        <f>AVERAGE(F2:F52)</f>
-        <v>0.10388</v>
-      </c>
-      <c r="G53" s="7">
-        <f>AVERAGE(G2:G52)</f>
-        <v>8.52</v>
-      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="7"/>
     </row>
   </sheetData>
   <sortState ref="A2:G52">

</xml_diff>